<commit_message>
working smooth so far
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1232,7 +1232,7 @@
         <v>Invoiced</v>
       </c>
       <c r="J17" t="str">
-        <v>Zenith bank</v>
+        <v>CASH</v>
       </c>
       <c r="K17">
         <v>10</v>
@@ -1244,19 +1244,419 @@
         <v>Bernard</v>
       </c>
       <c r="N17">
-        <v>343344</v>
+        <v>2324735</v>
       </c>
       <c r="O17" t="str">
         <v>253705</v>
       </c>
       <c r="P17" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>64bba574a7499d7733f537e3</v>
+      </c>
+      <c r="B18" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C18">
+        <v>4200673</v>
+      </c>
+      <c r="D18">
+        <v>1900</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45129.04207175926</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Cash payment</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J18" t="str">
+        <v>CASH</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N18">
+        <v>4200673</v>
+      </c>
+      <c r="O18" t="str">
+        <v>976105</v>
+      </c>
+      <c r="P18" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>64bc3de5863ca7a448d1955e</v>
+      </c>
+      <c r="B19" t="str">
+        <v>6405f77c1ec640bb7919b533</v>
+      </c>
+      <c r="C19">
+        <v>1884668</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45129.04207175926</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Cash payment</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J19" t="str">
+        <v>CASH</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M19" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N19">
+        <v>1884668</v>
+      </c>
+      <c r="O19" t="str">
+        <v>566965</v>
+      </c>
+      <c r="P19" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>64bc62d7250f0d99f9814523</v>
+      </c>
+      <c r="B20" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C20">
+        <v>1422049</v>
+      </c>
+      <c r="D20">
+        <v>1200</v>
+      </c>
+      <c r="E20" s="1">
+        <v>45131.04207175926</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Bank Payment</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J20" t="str">
+        <v>GT Bank</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20" t="str">
+        <v>64996a6f08c70837359160b9</v>
+      </c>
+      <c r="M20" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N20">
+        <v>1422049</v>
+      </c>
+      <c r="O20" t="str">
+        <v>519375</v>
+      </c>
+      <c r="P20" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>64bdb5afa815a7d13319bc28</v>
+      </c>
+      <c r="B21" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C21">
+        <v>20260</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>45131.04207175926</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Bank Payment</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J21" t="str">
+        <v>GT Bank</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M21" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N21">
+        <v>20260</v>
+      </c>
+      <c r="O21" t="str">
+        <v>98492</v>
+      </c>
+      <c r="P21" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>64bdd2d5344b2b124336df12</v>
+      </c>
+      <c r="B22" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C22">
+        <v>930494</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>45131.04207175926</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Cash payment</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J22" t="str">
+        <v>CASH</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M22" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N22">
+        <v>930494</v>
+      </c>
+      <c r="O22" t="str">
+        <v>325346</v>
+      </c>
+      <c r="P22" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>64be3289c3b8ea80b088774f</v>
+      </c>
+      <c r="B23" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C23">
+        <v>1395241</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="1">
+        <v>45131.04207175926</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Bank Payment</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J23" t="str">
+        <v>GT Bank</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M23" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N23">
+        <v>1395241</v>
+      </c>
+      <c r="O23" t="str">
+        <v>161058</v>
+      </c>
+      <c r="P23" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>64c03a836452e19bacfb6b82</v>
+      </c>
+      <c r="B24" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C24">
+        <v>28680</v>
+      </c>
+      <c r="D24">
+        <v>3000</v>
+      </c>
+      <c r="E24" s="1">
+        <v>45132.04207175926</v>
+      </c>
+      <c r="F24" t="str">
+        <v>Cash payment</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J24" t="str">
+        <v>CASH</v>
+      </c>
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M24" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N24">
+        <v>28680</v>
+      </c>
+      <c r="O24" t="str">
+        <v>989329</v>
+      </c>
+      <c r="P24" t="str">
+        <v>Approved</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>64c21fb6bd52a08c991a112a</v>
+      </c>
+      <c r="B25" t="str">
+        <v>640900b19a139999b1824b31</v>
+      </c>
+      <c r="C25">
+        <v>4209403</v>
+      </c>
+      <c r="D25">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="1">
+        <v>45138.04207175926</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Cash payment</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="str">
+        <v>Invoiced</v>
+      </c>
+      <c r="J25" t="str">
+        <v>GT Bank</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25" t="str">
+        <v>64a282ffb1d2b9bb36188d0c</v>
+      </c>
+      <c r="M25" t="str">
+        <v>Bernard</v>
+      </c>
+      <c r="N25">
+        <v>4209403</v>
+      </c>
+      <c r="O25" t="str">
+        <v>107491</v>
+      </c>
+      <c r="P25" t="str">
         <v>Approved</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>